<commit_message>
tabla excel hasta 16000 - maria
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 - MC.xlsx
+++ b/Docs/Tablas Lab 4 - MC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc/Documents/GitHub/EDA/LabSorts-S04-G04/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C2D05D-C99F-664D-8DDD-CC383C63A461}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25780" windowHeight="15580" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -142,6 +148,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -526,7 +541,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +628,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -652,7 +667,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,34 +679,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>637.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2713.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>10936.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>43601.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>179375.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +781,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -820,7 +820,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -832,34 +832,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>670.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2916.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10710.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>44929.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>186474.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,7 +933,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -987,7 +972,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,34 +984,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>37.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>85.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>192.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>431.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>1017.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,7 +1096,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1134,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1218,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1256,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1298,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1335,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1441,7 +1411,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1528,7 +1498,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1567,7 +1537,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,36 +1548,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1696,7 +1636,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1707,36 +1647,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1746,36 +1656,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1863,7 +1743,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1902,7 +1782,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,36 +1793,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2041,7 +1891,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +1929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +2013,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +2051,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2093,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2130,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2356,7 +2206,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,7 +2294,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2483,7 +2333,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2495,34 +2345,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>637.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2713.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>10936.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>43601.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>179375.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,7 +2447,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2651,7 +2486,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2662,36 +2497,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2790,7 +2595,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2633,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2712,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2750,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2792,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +2829,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3095,7 +2900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +2988,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3222,7 +3027,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3234,34 +3039,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>670.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2916.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10710.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>44929.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>186474.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,7 +3141,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3390,7 +3180,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3401,36 +3191,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3529,7 +3289,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3327,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3406,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3444,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3486,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3523,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3834,7 +3594,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,7 +3682,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3961,7 +3721,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3973,34 +3733,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>37.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>85.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>192.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>431.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>1017.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,7 +3835,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4129,7 +3874,7 @@
                   <c:v>256000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512000</c:v>
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4140,36 +3885,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4268,7 +3983,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4021,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,7 +4100,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4423,7 +4138,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4180,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4217,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7330,7 +7045,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7473,7 +7188,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8685893" cy="6293304"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7827,19 +7542,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,164 +7568,117 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4">
-        <v>10</v>
+      <c r="B2" s="5">
+        <v>637.6</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>670.63</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>37.69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>2713.14</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
+      <c r="C3" s="6">
+        <v>2916.61</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>85.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>10936.16</v>
       </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+      <c r="C4" s="7">
+        <v>10710.49</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>192.73</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>43601.07</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+      <c r="C5" s="6">
+        <v>44929.52</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>431.34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>179375.07</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+      <c r="C6" s="7">
+        <v>186474.09</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>1017.22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="4">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>375942</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8024,162 +7692,85 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>35</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
-      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="4">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
-      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>375942</v>
       </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A24" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8191,15 +7782,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -8410,21 +7992,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8443,11 +8026,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>